<commit_message>
New data format, additional column for valid street number
</commit_message>
<xml_diff>
--- a/doc/Locations.xlsx
+++ b/doc/Locations.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V004458\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="9672"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>PLZ</t>
   </si>
@@ -33,6 +28,9 @@
   </si>
   <si>
     <t>Strasse</t>
+  </si>
+  <si>
+    <t>Erste_Hausnummer</t>
   </si>
 </sst>
 </file>
@@ -341,7 +339,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -349,15 +347,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -367,6 +368,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>